<commit_message>
OrchestratorQueueName runtime arg now works
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="4530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="4530"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>C:\Users\rr523860\Documents\UiPath\Book Billing - Moving Jobs Ready to Bill\Dispatcher</t>
-  </si>
-  <si>
-    <t>BooksBillingReadyToMoveQ</t>
   </si>
   <si>
     <t>ErrorEmailAddress</t>
@@ -557,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -608,7 +605,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
@@ -622,7 +619,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -745,7 +742,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -758,10 +755,10 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2967,8 +2964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3012,10 +3009,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactored to make use of DateTime class
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -552,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z985"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -634,144 +634,60 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>31</v>
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>28</v>
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>31</v>
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>30</v>
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1725,21 +1641,9 @@
     <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B21" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>